<commit_message>
finished ML intro, ran couple more tests
</commit_message>
<xml_diff>
--- a/documents/ml_results.xlsx
+++ b/documents/ml_results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843555F7-664C-4698-9423-1ADDC7F6D2B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911C1821-5BA5-4FAC-B864-EB732821B0B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogisticRegression" sheetId="7" r:id="rId1"/>
@@ -17,9 +17,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DecisionTree!$A$1:$G$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">kNearestNeighbors!$A$1:$I$20</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LogisticRegression!$A$1:$F$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LogisticRegression!$A$1:$F$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NeuralNetwork!$A$1:$F$20</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RandomForest!$A$1:$G$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RandomForest!$A$1:$G$14</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="14">
   <si>
     <t>acc</t>
   </si>
@@ -413,11 +413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856F87AE-4138-43C4-AA25-4A1F756117CA}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,11 +650,17 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="2">
-        <v>0.64978931446167099</v>
+        <v>0.66306520447301598</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -666,11 +672,8 @@
       <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
       <c r="F14" s="2">
-        <v>0.64856031548808801</v>
+        <v>0.64978931446167099</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -679,23 +682,14 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2">
-        <v>0.64336070444600502</v>
+        <v>0.64856031548808801</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -710,8 +704,17 @@
       <c r="B16" t="s">
         <v>7</v>
       </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
       <c r="F16" s="2">
-        <v>0.64098373939819497</v>
+        <v>0.64336070444600502</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -721,13 +724,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" s="2">
-        <v>0.639943817189779</v>
+        <v>0.64098373939819497</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -737,22 +740,13 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2">
-        <v>0.63770190697423101</v>
+        <v>0.639943817189779</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -773,6 +767,9 @@
       <c r="D19" t="s">
         <v>9</v>
       </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
       <c r="F19" s="2">
         <v>0.63770190697423101</v>
       </c>
@@ -783,14 +780,21 @@
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2">
         <v>0.63770190697423101</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -798,12 +802,14 @@
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>8</v>
+      <c r="D21" t="s">
+        <v>10</v>
       </c>
       <c r="F21" s="2">
         <v>0.63770190697423101</v>
       </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -811,8 +817,8 @@
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E22" t="s">
-        <v>10</v>
+      <c r="B22" t="s">
+        <v>8</v>
       </c>
       <c r="F22" s="2">
         <v>0.63770190697423101</v>
@@ -824,8 +830,8 @@
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>7</v>
+      <c r="E23" t="s">
+        <v>10</v>
       </c>
       <c r="F23" s="2">
         <v>0.63770190697423101</v>
@@ -837,8 +843,8 @@
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>8</v>
+      <c r="B24" t="s">
+        <v>7</v>
       </c>
       <c r="F24" s="2">
         <v>0.63770190697423101</v>
@@ -850,8 +856,8 @@
       <c r="M24" s="2"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
-        <v>10</v>
+      <c r="A25" t="s">
+        <v>8</v>
       </c>
       <c r="F25" s="2">
         <v>0.63770190697423101</v>
@@ -866,9 +872,6 @@
       <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
       <c r="F26" s="2">
         <v>0.63770190697423101</v>
       </c>
@@ -885,9 +888,6 @@
       <c r="D27" t="s">
         <v>10</v>
       </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
       <c r="F27" s="2">
         <v>0.63770190697423101</v>
       </c>
@@ -898,8 +898,14 @@
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F28" s="2">
         <v>0.63770190697423101</v>
@@ -911,8 +917,8 @@
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>7</v>
+      <c r="E29" t="s">
+        <v>9</v>
       </c>
       <c r="F29" s="2">
         <v>0.63770190697423101</v>
@@ -924,8 +930,8 @@
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>11</v>
+      <c r="A30" t="s">
+        <v>7</v>
       </c>
       <c r="F30" s="2">
         <v>0.63770190697423101</v>
@@ -937,7 +943,7 @@
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="2">
@@ -953,9 +959,6 @@
       <c r="A32" t="s">
         <v>11</v>
       </c>
-      <c r="B32" t="s">
-        <v>11</v>
-      </c>
       <c r="F32" s="2">
         <v>0.63770190697423101</v>
       </c>
@@ -965,13 +968,29 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.63770190697423101</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F34" xr:uid="{EA4E2EBD-50AC-4C21-A6CC-933FC52BE30F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F34">
-      <sortCondition descending="1" ref="F1:F34"/>
+  <autoFilter ref="A1:F35" xr:uid="{EA4E2EBD-50AC-4C21-A6CC-933FC52BE30F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
+      <sortCondition descending="1" ref="F1:F35"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="F33:F1048576 I2:I32 F1">
+  <conditionalFormatting sqref="F34:F1048576 I2:I33 F1">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -995,7 +1014,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:M32 G4:G5 G20:H20">
+  <conditionalFormatting sqref="J2:M33 G4:G5 G21:H21">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -1391,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9B5DD6-B584-43B3-8608-5D97FAC5AE9C}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2106,11 +2125,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF53D2C2-1311-4DBA-8ECB-9DDB1922C746}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2172,10 +2191,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -2187,14 +2206,34 @@
         <v>10</v>
       </c>
       <c r="F3" s="2">
+        <v>0.69989465723083499</v>
+      </c>
+      <c r="G3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
         <v>0.69919237210307295</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F5" s="2"/>
@@ -2221,12 +2260,12 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E13" s="3"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E14" s="3"/>
       <c r="F14" s="2"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F15" s="2"/>
@@ -2243,10 +2282,13 @@
     <row r="19" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
     </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G13" xr:uid="{554AB7BA-2D8F-4083-9827-F05AEA390CA8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
-      <sortCondition descending="1" ref="F1:F13"/>
+  <autoFilter ref="A1:G14" xr:uid="{554AB7BA-2D8F-4083-9827-F05AEA390CA8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
+      <sortCondition descending="1" ref="F1:F14"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
added conclusion, almost finished writing analysis, only LinReg left
</commit_message>
<xml_diff>
--- a/documents/ml_results.xlsx
+++ b/documents/ml_results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66973DA8-F111-4C63-8540-2C8E062495D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14471C30-ECE6-4672-8B49-FA0DE84FD21B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogisticRegression" sheetId="7" r:id="rId1"/>
@@ -21,10 +21,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NeuralNetwork!$A$1:$F$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">RandomForest!$A$1:$G$14</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -409,9 +415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856F87AE-4138-43C4-AA25-4A1F756117CA}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -979,11 +985,6 @@
       <c r="M33" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F35" xr:uid="{EA4E2EBD-50AC-4C21-A6CC-933FC52BE30F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
-      <sortCondition descending="1" ref="F1:F35"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="F34:F1048576 I2:I33 F1">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -1028,9 +1029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE497B23-D95D-43E9-95EE-B256F7AC9097}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="A1:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1365,11 +1366,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G22" xr:uid="{8CD3A7FD-13A4-4FA4-B364-3B7526ED7D0B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G19">
-      <sortCondition descending="1" ref="G1:G22"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="G5:G1048576 G2">
     <cfRule type="colorScale" priority="6">
       <colorScale>
@@ -1440,8 +1436,8 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="A1:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2119,11 +2115,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G39" xr:uid="{ED5DE24A-2317-44E1-BEEC-F8431B04463A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G39">
-      <sortCondition descending="1" ref="G1:G39"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="J2:J35 G36:G1048576">
     <cfRule type="colorScale" priority="3">
       <colorScale>
@@ -2166,11 +2157,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF53D2C2-1311-4DBA-8ECB-9DDB1922C746}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2184,7 +2175,7 @@
     <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2207,7 +2198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2229,8 +2220,12 @@
       <c r="G2" s="2">
         <v>0.70015126141213302</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="2">
+        <f>G2-0.6366</f>
+        <v>6.3551261412132964E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2253,7 +2248,7 @@
         <v>0.69989465723083499</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2276,42 +2271,42 @@
         <v>0.69919237210307295</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.35">
@@ -2327,11 +2322,6 @@
       <c r="G20" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G14" xr:uid="{554AB7BA-2D8F-4083-9827-F05AEA390CA8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
-      <sortCondition descending="1" ref="G1:G14"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -2366,7 +2356,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2544,11 +2534,6 @@
       <c r="F20" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F20" xr:uid="{559C3605-73A4-4826-B2CA-BF302C974C6B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
-      <sortCondition descending="1" ref="F1:F20"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>

<commit_message>
updated data with linear regression results
</commit_message>
<xml_diff>
--- a/documents/ml_results.xlsx
+++ b/documents/ml_results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14471C30-ECE6-4672-8B49-FA0DE84FD21B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5053EACB-A79D-4E96-AB64-2DBDEE672958}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogisticRegression" sheetId="7" r:id="rId1"/>
@@ -13,10 +13,12 @@
     <sheet name="DecisionTree" sheetId="8" r:id="rId3"/>
     <sheet name="RandomForest" sheetId="10" r:id="rId4"/>
     <sheet name="NeuralNetwork" sheetId="5" r:id="rId5"/>
+    <sheet name="LinearRegression" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">DecisionTree!$A$1:$G$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">kNearestNeighbors!$A$1:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">LinearRegression!$A$1:$H$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LogisticRegression!$A$1:$F$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NeuralNetwork!$A$1:$F$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">RandomForest!$A$1:$G$14</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="16">
   <si>
     <t>d</t>
   </si>
@@ -76,6 +78,15 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>r^2</t>
+  </si>
+  <si>
+    <t>poly</t>
+  </si>
+  <si>
+    <t>intercept</t>
   </si>
 </sst>
 </file>
@@ -415,22 +426,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856F87AE-4138-43C4-AA25-4A1F756117CA}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -450,7 +461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -475,7 +486,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -497,7 +508,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -517,7 +528,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -537,7 +548,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -553,7 +564,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -569,7 +580,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -585,7 +596,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -604,7 +615,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>5</v>
       </c>
@@ -620,7 +631,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -636,7 +647,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>5</v>
       </c>
@@ -649,7 +660,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -668,7 +679,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>5</v>
       </c>
@@ -681,7 +692,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>5</v>
       </c>
@@ -697,7 +708,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -722,7 +733,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -738,7 +749,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -754,7 +765,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -779,7 +790,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -801,7 +812,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>8</v>
       </c>
@@ -816,7 +827,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -829,7 +840,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>8</v>
       </c>
@@ -842,7 +853,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -855,7 +866,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -868,7 +879,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>8</v>
       </c>
@@ -881,7 +892,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>8</v>
       </c>
@@ -897,7 +908,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>8</v>
       </c>
@@ -916,7 +927,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>5</v>
       </c>
@@ -929,7 +940,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -942,7 +953,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>4</v>
       </c>
@@ -955,7 +966,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -968,7 +979,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1034,18 +1045,18 @@
       <selection pane="bottomLeft" activeCell="G2" sqref="A1:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1099,7 @@
         <v>0.693114904651288</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1111,7 +1122,7 @@
         <v>0.69223704824158605</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1131,7 +1142,7 @@
         <v>0.691075576684133</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1165,7 @@
         <v>0.69094052185187105</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1171,7 +1182,7 @@
         <v>0.69068391767057402</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1191,7 +1202,7 @@
         <v>0.69046782993895495</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1208,7 +1219,7 @@
         <v>0.69013019285830002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1231,7 +1242,7 @@
         <v>0.68957646804602601</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1248,7 +1259,7 @@
         <v>0.68424180217168096</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1273,7 @@
         <v>0.68314785803036004</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1276,7 +1287,7 @@
         <v>0.68201339743935996</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>8</v>
       </c>
@@ -1287,7 +1298,7 @@
         <v>0.66344335800334897</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1301,7 +1312,7 @@
         <v>0.65904057047161102</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>8</v>
       </c>
@@ -1312,7 +1323,7 @@
         <v>0.64978931446167099</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1332,7 +1343,7 @@
         <v>0.64229377127113596</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1343,7 +1354,7 @@
         <v>0.63786397277294504</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1354,7 +1365,7 @@
         <v>0.63783696180649296</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1440,18 +1451,18 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="A1:G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1474,7 +1485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1510,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1524,7 +1535,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1546,7 +1557,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1568,7 +1579,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1593,7 +1604,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1618,7 +1629,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1643,7 +1654,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1665,7 +1676,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1687,7 +1698,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1706,7 +1717,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1724,7 +1735,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1743,7 +1754,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1762,7 +1773,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1778,7 +1789,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1794,7 +1805,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1810,7 +1821,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -1826,7 +1837,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1842,7 +1853,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -1858,7 +1869,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -1873,7 +1884,7 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>8</v>
       </c>
@@ -1891,7 +1902,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>5</v>
       </c>
@@ -1910,7 +1921,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>8</v>
       </c>
@@ -1926,7 +1937,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>8</v>
       </c>
@@ -1939,7 +1950,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>5</v>
       </c>
@@ -1952,7 +1963,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1967,7 +1978,7 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1983,7 +1994,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1998,7 +2009,7 @@
       </c>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>8</v>
       </c>
@@ -2010,7 +2021,7 @@
       </c>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>5</v>
       </c>
@@ -2022,7 +2033,7 @@
       </c>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>4</v>
       </c>
@@ -2034,7 +2045,7 @@
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -2046,7 +2057,7 @@
       </c>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -2058,7 +2069,7 @@
       </c>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2070,7 +2081,7 @@
       </c>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2092,7 @@
         <v>0.64336070444600502</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -2092,7 +2103,7 @@
         <v>0.637715412457457</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>8</v>
       </c>
@@ -2103,7 +2114,7 @@
         <v>0.63770190697423101</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>5</v>
       </c>
@@ -2164,18 +2175,18 @@
       <selection pane="bottomLeft" activeCell="L7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2198,7 +2209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2225,7 +2236,7 @@
         <v>6.3551261412132964E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2248,7 +2259,7 @@
         <v>0.69989465723083499</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2271,54 +2282,54 @@
         <v>0.69919237210307295</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G20" s="2"/>
     </row>
   </sheetData>
@@ -2356,21 +2367,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="A1:F8"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2391,7 +2402,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2411,7 +2422,7 @@
         <v>0.68110000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2425,7 +2436,7 @@
         <v>0.67179999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2445,7 +2456,7 @@
         <v>0.67059999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -2459,7 +2470,7 @@
         <v>0.67030000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -2467,7 +2478,7 @@
         <v>0.66659999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2487,7 +2498,7 @@
         <v>0.64480000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -2495,42 +2506,42 @@
         <v>0.64049999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" s="2"/>
     </row>
   </sheetData>
@@ -2560,4 +2571,296 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B0459B-4AA4-4A9B-B102-C6EA54B09617}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.3445023293411001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.30902556069979E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7.0428815412892903E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5.2219445205473596E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.4512007073468299E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8.7172993309292401E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7.6460973285485902E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.6598115442534301E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6.2015461568365406E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5.1597522955692999E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.9512897379846401E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2.9512897379846401E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-6.4120788771937498E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="2">
+        <v>-6.4120788771937498E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2">
+        <v>-8.9750663002159392E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="5">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2">
+        <v>-131.08493123036999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H24" xr:uid="{BF1A242F-142E-4E31-9516-0E41F5F3B72B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H24">
+      <sortCondition descending="1" ref="H1:H24"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="H2:H17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new results with PCA
</commit_message>
<xml_diff>
--- a/documents/ml_results.xlsx
+++ b/documents/ml_results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0199B902-9047-42FF-B247-A407FC8C8279}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A61D98A-0027-4CDC-AD95-1527D32BAEA8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogisticRegression" sheetId="7" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">DecisionTree!$A$1:$G$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">kNearestNeighbors!$A$1:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">kNearestNeighbors!$A$1:$H$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">LinearRegression!$A$1:$G$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LogisticRegression!$A$1:$F$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NeuralNetwork!$A$1:$F$20</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="16">
   <si>
     <t>d</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>poly</t>
+  </si>
+  <si>
+    <t>pca</t>
   </si>
 </sst>
 </file>
@@ -425,17 +428,17 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1035,25 +1038,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE497B23-D95D-43E9-95EE-B256F7AC9097}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="A1:G19"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1070,13 +1074,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1089,14 +1096,14 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>95</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>0.693114904651288</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1104,278 +1111,324 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>65</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.69257468532223998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4">
         <v>79</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H4" s="2">
         <v>0.69223704824158605</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5">
         <v>49</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H5" s="2">
         <v>0.691075576684133</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6">
         <v>47</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H6" s="2">
         <v>0.69094052185187105</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
         <v>49</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H7" s="2">
         <v>0.69068391767057402</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8">
         <v>47</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H8" s="2">
         <v>0.69046782993895495</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9">
         <v>47</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H9" s="2">
         <v>0.69013019285830002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10">
         <v>41</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>0.68957646804602601</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11">
         <v>49</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H11" s="2">
         <v>0.68424180217168096</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12">
         <v>49</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>0.68314785803036004</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13">
         <v>49</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>0.68201339743935996</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14">
         <v>45</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>0.66344335800334897</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>95</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.66040462427745605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16">
         <v>47</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H16" s="2">
         <v>0.65904057047161102</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17">
         <v>15</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H17" s="2">
         <v>0.64978931446167099</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>49</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.64229377127113596</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17">
-        <v>45</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0.63786397277294504</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="F18">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>49</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.64229377127113596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19">
         <v>45</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H19" s="2">
+        <v>0.63786397277294504</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>45</v>
+      </c>
+      <c r="H20" s="2">
         <v>0.63783696180649296</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21">
         <v>45</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H21" s="2">
         <v>0.63783696180649296</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G5:G1048576 G2">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="H23:H1048576">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1386,8 +1439,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="H1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1398,8 +1451,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="H25:H1048576 G1">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1410,20 +1463,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G23:G1048576 F1">
-    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1445,18 +1486,18 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="A1:G39"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2169,18 +2210,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2228,10 +2270,7 @@
       <c r="G2" s="2">
         <v>0.70015126141213302</v>
       </c>
-      <c r="H2" s="2">
-        <f>G2-0.6366</f>
-        <v>6.3551261412132964E-2</v>
-      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2369,12 +2408,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2574,19 +2613,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B0459B-4AA4-4A9B-B102-C6EA54B09617}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>